<commit_message>
pop up error if bad start
</commit_message>
<xml_diff>
--- a/exceltestdata/settings.xlsx
+++ b/exceltestdata/settings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6915"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6915" firstSheet="2" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Общие настройки" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13934" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14002" uniqueCount="69">
   <si>
     <t>Место</t>
   </si>
@@ -708,7 +708,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -786,6 +786,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2280,10 +2283,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2329,196 +2332,166 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="C7" s="27">
         <v>1</v>
       </c>
       <c r="D7" s="28" t="str">
-        <f>IF(C7=1, "Выбрана сплошная рассадка", IF(C7=2, "Выбрана рассадка через место","Ошибка, надо выбрать 1 или 2"))</f>
-        <v>Выбрана сплошная рассадка</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <f>IF(NOT(C7=""),IF(C7=0,"В целях рассадки участники из 8 и 9 классов равны одноклассникам",IF(C7=1,"Участники из 8 и 9 классов могут сидеть рядом","Ошибка, надо выбрать 0 или 1")),"Необходимо ввести значение")</f>
+        <v>Участники из 8 и 9 классов могут сидеть рядом</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="B8" s="29" t="s">
-        <v>25</v>
+        <v>32</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>48</v>
       </c>
       <c r="C8" s="27">
         <v>1</v>
       </c>
       <c r="D8" s="28" t="str">
-        <f>IF(C8=1,"Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается",IF(C8=2,"Участники сидят через ряд, каждый второй ряд свободен",IF(C8=3,"Участники сидят два ряда через один, каждый третий ряд свободен","Ошибка, надо выбрать из 1, 2, 3")))</f>
-        <v>Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается</v>
+        <f>IF(NOT(C8=""),IF(C8=0,"В целях рассадки участники из 8 и 10 классов равны одноклассникам",IF(C8=1,"Участники из 8 и 10 классов могут сидеть рядом","Ошибка, надо выбрать 0 или 1")),"Необходимо ввести значение")</f>
+        <v>Участники из 8 и 10 классов могут сидеть рядом</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C9" s="27">
         <v>1</v>
       </c>
       <c r="D9" s="28" t="str">
-        <f>IF(NOT(C9=""),IF(C9=0,"В целях рассадки участники из 8 и 9 классов равны одноклассникам",IF(C9=1,"Участники из 8 и 9 классов могут сидеть рядом","Ошибка, надо выбрать 0 или 1")),"Необходимо ввести значение")</f>
-        <v>Участники из 8 и 9 классов могут сидеть рядом</v>
+        <f>IF(NOT(C9=""),IF(C9=0,"В целях рассадки участники из 8 и 11 классов равны одноклассникам",IF(C9=1,"Участники из 8 и 11 классов могут сидеть рядом","Ошибка, надо выбрать 0 или 1")),"Необходимо ввести значение")</f>
+        <v>Участники из 8 и 11 классов могут сидеть рядом</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C10" s="27">
         <v>1</v>
       </c>
       <c r="D10" s="28" t="str">
-        <f>IF(NOT(C10=""),IF(C10=0,"В целях рассадки участники из 8 и 10 классов равны одноклассникам",IF(C10=1,"Участники из 8 и 10 классов могут сидеть рядом","Ошибка, надо выбрать 0 или 1")),"Необходимо ввести значение")</f>
-        <v>Участники из 8 и 10 классов могут сидеть рядом</v>
+        <f>IF(NOT(C10=""),IF(C10=0,"В целях рассадки участники из 9 и 10 классов равны одноклассникам",IF(C10=1,"Участники из 9 и 10 классов могут сидеть рядом","Ошибка, надо выбрать 0 или 1")),"Необходимо ввести значение")</f>
+        <v>Участники из 9 и 10 классов могут сидеть рядом</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C11" s="27">
         <v>1</v>
       </c>
       <c r="D11" s="28" t="str">
-        <f>IF(NOT(C11=""),IF(C11=0,"В целях рассадки участники из 8 и 11 классов равны одноклассникам",IF(C11=1,"Участники из 8 и 11 классов могут сидеть рядом","Ошибка, надо выбрать 0 или 1")),"Необходимо ввести значение")</f>
-        <v>Участники из 8 и 11 классов могут сидеть рядом</v>
+        <f>IF(NOT(C11=""),IF(C11=0,"В целях рассадки участники из 9 и 11 классов равны одноклассникам",IF(C11=1,"Участники из 9 и 11 классов могут сидеть рядом","Ошибка, надо выбрать 0 или 1")),"Необходимо ввести значение")</f>
+        <v>Участники из 9 и 11 классов могут сидеть рядом</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C12" s="27">
         <v>1</v>
       </c>
       <c r="D12" s="28" t="str">
-        <f>IF(NOT(C12=""),IF(C12=0,"В целях рассадки участники из 9 и 10 классов равны одноклассникам",IF(C12=1,"Участники из 9 и 10 классов могут сидеть рядом","Ошибка, надо выбрать 0 или 1")),"Необходимо ввести значение")</f>
-        <v>Участники из 9 и 10 классов могут сидеть рядом</v>
+        <f>IF(NOT(C12=""),IF(C12=0,"В целях рассадки участники из 10 и 11 классов равны одноклассникам",IF(C12=1,"Участники из 10 и 11 классов могут сидеть рядом","Ошибка, надо выбрать 0 или 1")),"Необходимо ввести значение")</f>
+        <v>Участники из 10 и 11 классов могут сидеть рядом</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C13" s="27">
         <v>1</v>
       </c>
       <c r="D13" s="28" t="str">
-        <f>IF(NOT(C13=""),IF(C13=0,"В целях рассадки участники из 9 и 11 классов равны одноклассникам",IF(C13=1,"Участники из 9 и 11 классов могут сидеть рядом","Ошибка, надо выбрать 0 или 1")),"Необходимо ввести значение")</f>
-        <v>Участники из 9 и 11 классов могут сидеть рядом</v>
+        <f>IF(NOT(C13=""),IF(C13=0,"Участники из одной школы не сидят рядом. Что такое РЯДОМ настраивается ниже",IF(C13=1,"Участники из одной школы могут сидеть рядом","Ошибка, надо выбрать 1 или 2")),"Необходимо ввести значение")</f>
+        <v>Участники из одной школы могут сидеть рядом</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C14" s="27">
         <v>1</v>
       </c>
       <c r="D14" s="28" t="str">
-        <f>IF(NOT(C14=""),IF(C14=0,"В целях рассадки участники из 10 и 11 классов равны одноклассникам",IF(C14=1,"Участники из 10 и 11 классов могут сидеть рядом","Ошибка, надо выбрать 0 или 1")),"Необходимо ввести значение")</f>
-        <v>Участники из 10 и 11 классов могут сидеть рядом</v>
+        <f>IF(NOT(C14=""),IF(C14=0,"Участники из одного города не сидят рядом. Что такое РЯДОМ настраивается ниже",IF(C14=1,"Участники из одного города могут сидеть рядом","Ошибка, надо выбрать 1 или 2")),"Необходимо ввести значение")</f>
+        <v>Участники из одного города могут сидеть рядом</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="C15" s="27">
         <v>1</v>
       </c>
       <c r="D15" s="28" t="str">
-        <f>IF(NOT(C15=""),IF(C15=0,"Участники из одной школы не сидят рядом. Что такое РЯДОМ настраивается ниже",IF(C15=1,"Участники из одной школы могут сидеть рядом","Ошибка, надо выбрать 1 или 2")),"Необходимо ввести значение")</f>
-        <v>Участники из одной школы могут сидеть рядом</v>
+        <f>IF(NOT(C15=""),IF(C15=1,"Командные участники сидят в одной аудитории",IF(C15=0,"Командные участники могут сидеть в разных аудиториях","Ошибка, надо выбрать 1 или 0")),"Необходимо ввести значение")</f>
+        <v>Командные участники сидят в одной аудитории</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C16" s="27">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="D16" s="28" t="str">
-        <f>IF(NOT(C16=""),IF(C16=0,"Участники из одного города не сидят рядом. Что такое РЯДОМ настраивается ниже",IF(C16=1,"Участники из одного города могут сидеть рядом","Ошибка, надо выбрать 1 или 2")),"Необходимо ввести значение")</f>
-        <v>Участники из одного города могут сидеть рядом</v>
+        <f>IF(AND(C16&gt;0,C16&lt;=1),CONCATENATE("Максимальная доля командников - ", C16*100, "%"),"Необходимо ввести число больше 0 и до 1")</f>
+        <v>Максимальная доля командников - 80%</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C17" s="27">
         <v>1</v>
       </c>
       <c r="D17" s="28" t="str">
-        <f>IF(NOT(C17=""),IF(C17=1,"Командные участники сидят в одной аудитории",IF(C17=0,"Командные участники могут сидеть в разных аудиториях","Ошибка, надо выбрать 1 или 0")),"Необходимо ввести значение")</f>
-        <v>Командные участники сидят в одной аудитории</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="27">
-        <v>0.8</v>
-      </c>
-      <c r="D18" s="28" t="str">
-        <f>IF(AND(C18&gt;0,C18&lt;=1),CONCATENATE("Максимальная доля командников - ", C18*100, "%"),"Необходимо ввести число больше 0 и до 1")</f>
-        <v>Максимальная доля командников - 80%</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" s="27">
-        <v>1</v>
-      </c>
-      <c r="D19" s="28" t="str">
-        <f>IF(NOT(C19=""),IF(C19=0,"Файл отладки создан не будет",IF(C19=1,"Будет создан файл отладки debug.txt","Ошибка, надо выбрать 0 или 1")),"Необходимо ввести значение")</f>
+        <f>IF(NOT(C17=""),IF(C17=0,"Файл отладки создан не будет",IF(C17=1,"Будет создан файл отладки debug.txt","Ошибка, надо выбрать 0 или 1")),"Необходимо ввести значение")</f>
         <v>Будет создан файл отладки debug.txt</v>
       </c>
     </row>
@@ -2533,7 +2506,7 @@
   <dimension ref="A3:AP35"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C16" sqref="C16:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3034,11 +3007,37 @@
       </c>
     </row>
     <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="29">
+        <v>1</v>
+      </c>
+      <c r="F16" s="44" t="str">
+        <f>IF(E16=1, "Выбрана сплошная рассадка", IF(E16=2, "Выбрана рассадка через место","Ошибка, надо выбрать 1 или 2"))</f>
+        <v>Выбрана сплошная рассадка</v>
+      </c>
       <c r="H16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:42" ht="60" x14ac:dyDescent="0.25">
+      <c r="C17" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="29">
+        <v>1</v>
+      </c>
+      <c r="F17" s="44" t="str">
+        <f>IF(E17=1,"Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается",IF(E17=2,"Участники сидят через ряд, каждый второй ряд свободен",IF(E17=3,"Участники сидят два ряда через один, каждый третий ряд свободен","Ошибка, надо выбрать из 1, 2, 3")))</f>
+        <v>Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается</v>
+      </c>
       <c r="I17" s="38" t="s">
         <v>0</v>
       </c>
@@ -3142,7 +3141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I18" s="31" t="s">
         <v>0</v>
       </c>
@@ -3246,7 +3245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I19" s="31" t="s">
         <v>0</v>
       </c>
@@ -3350,7 +3349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I20" s="31" t="s">
         <v>0</v>
       </c>
@@ -3454,7 +3453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I21" s="31" t="s">
         <v>0</v>
       </c>
@@ -3558,7 +3557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I22" s="31" t="s">
         <v>0</v>
       </c>
@@ -3662,7 +3661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I23" s="31" t="s">
         <v>0</v>
       </c>
@@ -3766,7 +3765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I24" s="31" t="s">
         <v>0</v>
       </c>
@@ -3870,7 +3869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I25" s="31" t="s">
         <v>0</v>
       </c>
@@ -3974,7 +3973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I26" s="31" t="s">
         <v>1</v>
       </c>
@@ -4078,7 +4077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I27" s="31" t="s">
         <v>1</v>
       </c>
@@ -4182,7 +4181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I28" s="31" t="s">
         <v>1</v>
       </c>
@@ -4286,7 +4285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I29" s="31" t="s">
         <v>1</v>
       </c>
@@ -4390,7 +4389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I30" s="31" t="s">
         <v>1</v>
       </c>
@@ -4494,7 +4493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I31" s="31" t="s">
         <v>1</v>
       </c>
@@ -4598,7 +4597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I32" s="31" t="s">
         <v>1</v>
       </c>
@@ -5068,7 +5067,7 @@
   <dimension ref="A3:AP35"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C16" sqref="C16:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5569,11 +5568,37 @@
       </c>
     </row>
     <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="29">
+        <v>1</v>
+      </c>
+      <c r="F16" s="44" t="str">
+        <f>IF(E16=1, "Выбрана сплошная рассадка", IF(E16=2, "Выбрана рассадка через место","Ошибка, надо выбрать 1 или 2"))</f>
+        <v>Выбрана сплошная рассадка</v>
+      </c>
       <c r="H16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:42" ht="60" x14ac:dyDescent="0.25">
+      <c r="C17" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="29">
+        <v>1</v>
+      </c>
+      <c r="F17" s="44" t="str">
+        <f>IF(E17=1,"Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается",IF(E17=2,"Участники сидят через ряд, каждый второй ряд свободен",IF(E17=3,"Участники сидят два ряда через один, каждый третий ряд свободен","Ошибка, надо выбрать из 1, 2, 3")))</f>
+        <v>Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается</v>
+      </c>
       <c r="I17" s="38" t="s">
         <v>0</v>
       </c>
@@ -5677,7 +5702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I18" s="31" t="s">
         <v>0</v>
       </c>
@@ -5781,7 +5806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I19" s="31" t="s">
         <v>0</v>
       </c>
@@ -5885,7 +5910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I20" s="31" t="s">
         <v>0</v>
       </c>
@@ -5989,7 +6014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I21" s="31" t="s">
         <v>0</v>
       </c>
@@ -6093,7 +6118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I22" s="31" t="s">
         <v>0</v>
       </c>
@@ -6197,7 +6222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I23" s="31" t="s">
         <v>0</v>
       </c>
@@ -6301,7 +6326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I24" s="31" t="s">
         <v>0</v>
       </c>
@@ -6405,7 +6430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I25" s="31" t="s">
         <v>0</v>
       </c>
@@ -6509,7 +6534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I26" s="31" t="s">
         <v>1</v>
       </c>
@@ -6613,7 +6638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I27" s="31" t="s">
         <v>1</v>
       </c>
@@ -6717,7 +6742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I28" s="31" t="s">
         <v>1</v>
       </c>
@@ -6821,7 +6846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I29" s="31" t="s">
         <v>1</v>
       </c>
@@ -6925,7 +6950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I30" s="31" t="s">
         <v>1</v>
       </c>
@@ -7029,7 +7054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I31" s="31" t="s">
         <v>1</v>
       </c>
@@ -7133,7 +7158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I32" s="31" t="s">
         <v>1</v>
       </c>
@@ -7603,7 +7628,7 @@
   <dimension ref="A3:AP35"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C16" sqref="C16:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8104,11 +8129,37 @@
       </c>
     </row>
     <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="29">
+        <v>1</v>
+      </c>
+      <c r="F16" s="44" t="str">
+        <f>IF(E16=1, "Выбрана сплошная рассадка", IF(E16=2, "Выбрана рассадка через место","Ошибка, надо выбрать 1 или 2"))</f>
+        <v>Выбрана сплошная рассадка</v>
+      </c>
       <c r="H16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:42" ht="60" x14ac:dyDescent="0.25">
+      <c r="C17" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="29">
+        <v>1</v>
+      </c>
+      <c r="F17" s="44" t="str">
+        <f>IF(E17=1,"Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается",IF(E17=2,"Участники сидят через ряд, каждый второй ряд свободен",IF(E17=3,"Участники сидят два ряда через один, каждый третий ряд свободен","Ошибка, надо выбрать из 1, 2, 3")))</f>
+        <v>Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается</v>
+      </c>
       <c r="I17" s="38" t="s">
         <v>0</v>
       </c>
@@ -8212,7 +8263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I18" s="31" t="s">
         <v>0</v>
       </c>
@@ -8316,7 +8367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I19" s="31" t="s">
         <v>0</v>
       </c>
@@ -8420,7 +8471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I20" s="31" t="s">
         <v>0</v>
       </c>
@@ -8524,7 +8575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I21" s="31" t="s">
         <v>0</v>
       </c>
@@ -8628,7 +8679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I22" s="31" t="s">
         <v>0</v>
       </c>
@@ -8732,7 +8783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I23" s="31" t="s">
         <v>0</v>
       </c>
@@ -8836,7 +8887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I24" s="31" t="s">
         <v>0</v>
       </c>
@@ -8940,7 +8991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I25" s="31" t="s">
         <v>0</v>
       </c>
@@ -9044,7 +9095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I26" s="31" t="s">
         <v>0</v>
       </c>
@@ -9148,7 +9199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I27" s="31" t="s">
         <v>0</v>
       </c>
@@ -9252,7 +9303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I28" s="31" t="s">
         <v>1</v>
       </c>
@@ -9356,7 +9407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I29" s="31" t="s">
         <v>1</v>
       </c>
@@ -9460,7 +9511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I30" s="31" t="s">
         <v>1</v>
       </c>
@@ -9564,7 +9615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I31" s="31" t="s">
         <v>1</v>
       </c>
@@ -9668,7 +9719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I32" s="31" t="s">
         <v>1</v>
       </c>
@@ -10138,7 +10189,7 @@
   <dimension ref="A3:AP35"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C16" sqref="C16:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10639,11 +10690,37 @@
       </c>
     </row>
     <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="29">
+        <v>1</v>
+      </c>
+      <c r="F16" s="44" t="str">
+        <f>IF(E16=1, "Выбрана сплошная рассадка", IF(E16=2, "Выбрана рассадка через место","Ошибка, надо выбрать 1 или 2"))</f>
+        <v>Выбрана сплошная рассадка</v>
+      </c>
       <c r="H16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:42" ht="60" x14ac:dyDescent="0.25">
+      <c r="C17" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="29">
+        <v>1</v>
+      </c>
+      <c r="F17" s="44" t="str">
+        <f>IF(E17=1,"Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается",IF(E17=2,"Участники сидят через ряд, каждый второй ряд свободен",IF(E17=3,"Участники сидят два ряда через один, каждый третий ряд свободен","Ошибка, надо выбрать из 1, 2, 3")))</f>
+        <v>Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается</v>
+      </c>
       <c r="I17" s="38" t="s">
         <v>0</v>
       </c>
@@ -10747,7 +10824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I18" s="31" t="s">
         <v>0</v>
       </c>
@@ -10851,7 +10928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I19" s="31" t="s">
         <v>0</v>
       </c>
@@ -10955,7 +11032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I20" s="31" t="s">
         <v>0</v>
       </c>
@@ -11059,7 +11136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I21" s="31" t="s">
         <v>0</v>
       </c>
@@ -11163,7 +11240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I22" s="31" t="s">
         <v>0</v>
       </c>
@@ -11267,7 +11344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I23" s="31" t="s">
         <v>0</v>
       </c>
@@ -11371,7 +11448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I24" s="31" t="s">
         <v>0</v>
       </c>
@@ -11475,7 +11552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I25" s="31" t="s">
         <v>0</v>
       </c>
@@ -11579,7 +11656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I26" s="31" t="s">
         <v>1</v>
       </c>
@@ -11683,7 +11760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I27" s="31" t="s">
         <v>1</v>
       </c>
@@ -11787,7 +11864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I28" s="31" t="s">
         <v>1</v>
       </c>
@@ -11891,7 +11968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I29" s="31" t="s">
         <v>1</v>
       </c>
@@ -11995,7 +12072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I30" s="31" t="s">
         <v>1</v>
       </c>
@@ -12099,7 +12176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I31" s="31" t="s">
         <v>1</v>
       </c>
@@ -12203,7 +12280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I32" s="31" t="s">
         <v>1</v>
       </c>
@@ -12673,7 +12750,7 @@
   <dimension ref="A3:AP35"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C16" sqref="C16:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13174,11 +13251,37 @@
       </c>
     </row>
     <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="29">
+        <v>1</v>
+      </c>
+      <c r="F16" s="44" t="str">
+        <f>IF(E16=1, "Выбрана сплошная рассадка", IF(E16=2, "Выбрана рассадка через место","Ошибка, надо выбрать 1 или 2"))</f>
+        <v>Выбрана сплошная рассадка</v>
+      </c>
       <c r="H16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:42" ht="60" x14ac:dyDescent="0.25">
+      <c r="C17" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="29">
+        <v>1</v>
+      </c>
+      <c r="F17" s="44" t="str">
+        <f>IF(E17=1,"Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается",IF(E17=2,"Участники сидят через ряд, каждый второй ряд свободен",IF(E17=3,"Участники сидят два ряда через один, каждый третий ряд свободен","Ошибка, надо выбрать из 1, 2, 3")))</f>
+        <v>Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается</v>
+      </c>
       <c r="I17" s="38" t="s">
         <v>0</v>
       </c>
@@ -13282,7 +13385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I18" s="31" t="s">
         <v>0</v>
       </c>
@@ -13386,7 +13489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I19" s="31" t="s">
         <v>0</v>
       </c>
@@ -13490,7 +13593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I20" s="31" t="s">
         <v>0</v>
       </c>
@@ -13594,7 +13697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I21" s="31" t="s">
         <v>0</v>
       </c>
@@ -13698,7 +13801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I22" s="31" t="s">
         <v>0</v>
       </c>
@@ -13802,7 +13905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I23" s="31" t="s">
         <v>0</v>
       </c>
@@ -13906,7 +14009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I24" s="31" t="s">
         <v>0</v>
       </c>
@@ -14010,7 +14113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I25" s="31" t="s">
         <v>0</v>
       </c>
@@ -14114,7 +14217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I26" s="31" t="s">
         <v>0</v>
       </c>
@@ -14218,7 +14321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I27" s="31" t="s">
         <v>1</v>
       </c>
@@ -14322,7 +14425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I28" s="31" t="s">
         <v>1</v>
       </c>
@@ -14426,7 +14529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I29" s="31" t="s">
         <v>1</v>
       </c>
@@ -14530,7 +14633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I30" s="31" t="s">
         <v>1</v>
       </c>
@@ -14634,7 +14737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I31" s="31" t="s">
         <v>1</v>
       </c>
@@ -14738,7 +14841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I32" s="31" t="s">
         <v>1</v>
       </c>
@@ -15208,7 +15311,7 @@
   <dimension ref="A3:AP35"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C16" sqref="C16:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15709,11 +15812,37 @@
       </c>
     </row>
     <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="29">
+        <v>1</v>
+      </c>
+      <c r="F16" s="44" t="str">
+        <f>IF(E16=1, "Выбрана сплошная рассадка", IF(E16=2, "Выбрана рассадка через место","Ошибка, надо выбрать 1 или 2"))</f>
+        <v>Выбрана сплошная рассадка</v>
+      </c>
       <c r="H16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:42" ht="60" x14ac:dyDescent="0.25">
+      <c r="C17" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="29">
+        <v>1</v>
+      </c>
+      <c r="F17" s="44" t="str">
+        <f>IF(E17=1,"Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается",IF(E17=2,"Участники сидят через ряд, каждый второй ряд свободен",IF(E17=3,"Участники сидят два ряда через один, каждый третий ряд свободен","Ошибка, надо выбрать из 1, 2, 3")))</f>
+        <v>Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается</v>
+      </c>
       <c r="I17" s="38" t="s">
         <v>0</v>
       </c>
@@ -15817,7 +15946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I18" s="31" t="s">
         <v>0</v>
       </c>
@@ -15921,7 +16050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I19" s="31" t="s">
         <v>0</v>
       </c>
@@ -16025,7 +16154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I20" s="31" t="s">
         <v>0</v>
       </c>
@@ -16129,7 +16258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I21" s="31" t="s">
         <v>0</v>
       </c>
@@ -16233,7 +16362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I22" s="31" t="s">
         <v>0</v>
       </c>
@@ -16337,7 +16466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I23" s="31" t="s">
         <v>0</v>
       </c>
@@ -16441,7 +16570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I24" s="31" t="s">
         <v>1</v>
       </c>
@@ -16545,7 +16674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I25" s="31" t="s">
         <v>1</v>
       </c>
@@ -16649,7 +16778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I26" s="31" t="s">
         <v>1</v>
       </c>
@@ -16753,7 +16882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I27" s="31" t="s">
         <v>1</v>
       </c>
@@ -16857,7 +16986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I28" s="31" t="s">
         <v>1</v>
       </c>
@@ -16961,7 +17090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I29" s="31" t="s">
         <v>1</v>
       </c>
@@ -17065,7 +17194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I30" s="31" t="s">
         <v>1</v>
       </c>
@@ -17169,7 +17298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I31" s="31" t="s">
         <v>1</v>
       </c>
@@ -17273,7 +17402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I32" s="31" t="s">
         <v>1</v>
       </c>
@@ -17743,7 +17872,7 @@
   <dimension ref="A3:AP35"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C16" sqref="C16:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18244,11 +18373,37 @@
       </c>
     </row>
     <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="29">
+        <v>1</v>
+      </c>
+      <c r="F16" s="44" t="str">
+        <f>IF(E16=1, "Выбрана сплошная рассадка", IF(E16=2, "Выбрана рассадка через место","Ошибка, надо выбрать 1 или 2"))</f>
+        <v>Выбрана сплошная рассадка</v>
+      </c>
       <c r="H16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:42" ht="60" x14ac:dyDescent="0.25">
+      <c r="C17" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="29">
+        <v>1</v>
+      </c>
+      <c r="F17" s="44" t="str">
+        <f>IF(E17=1,"Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается",IF(E17=2,"Участники сидят через ряд, каждый второй ряд свободен",IF(E17=3,"Участники сидят два ряда через один, каждый третий ряд свободен","Ошибка, надо выбрать из 1, 2, 3")))</f>
+        <v>Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается</v>
+      </c>
       <c r="I17" s="31" t="s">
         <v>0</v>
       </c>
@@ -18352,7 +18507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I18" s="31" t="s">
         <v>0</v>
       </c>
@@ -18456,7 +18611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I19" s="31" t="s">
         <v>0</v>
       </c>
@@ -18560,7 +18715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I20" s="31" t="s">
         <v>0</v>
       </c>
@@ -18664,7 +18819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I21" s="31" t="s">
         <v>0</v>
       </c>
@@ -18768,7 +18923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I22" s="31" t="s">
         <v>0</v>
       </c>
@@ -18872,7 +19027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I23" s="31" t="s">
         <v>0</v>
       </c>
@@ -18976,7 +19131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I24" s="31" t="s">
         <v>1</v>
       </c>
@@ -19080,7 +19235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I25" s="31" t="s">
         <v>1</v>
       </c>
@@ -19184,7 +19339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I26" s="31" t="s">
         <v>1</v>
       </c>
@@ -19288,7 +19443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I27" s="31" t="s">
         <v>1</v>
       </c>
@@ -19392,7 +19547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I28" s="31" t="s">
         <v>1</v>
       </c>
@@ -19496,7 +19651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I29" s="31" t="s">
         <v>1</v>
       </c>
@@ -19600,7 +19755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I30" s="31" t="s">
         <v>1</v>
       </c>
@@ -19704,7 +19859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I31" s="31" t="s">
         <v>1</v>
       </c>
@@ -19808,7 +19963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I32" s="31" t="s">
         <v>1</v>
       </c>
@@ -20278,7 +20433,7 @@
   <dimension ref="A3:AP35"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C16" sqref="C16:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20779,11 +20934,37 @@
       </c>
     </row>
     <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="29">
+        <v>1</v>
+      </c>
+      <c r="F16" s="44" t="str">
+        <f>IF(E16=1, "Выбрана сплошная рассадка", IF(E16=2, "Выбрана рассадка через место","Ошибка, надо выбрать 1 или 2"))</f>
+        <v>Выбрана сплошная рассадка</v>
+      </c>
       <c r="H16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:42" ht="60" x14ac:dyDescent="0.25">
+      <c r="C17" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="29">
+        <v>1</v>
+      </c>
+      <c r="F17" s="44" t="str">
+        <f>IF(E17=1,"Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается",IF(E17=2,"Участники сидят через ряд, каждый второй ряд свободен",IF(E17=3,"Участники сидят два ряда через один, каждый третий ряд свободен","Ошибка, надо выбрать из 1, 2, 3")))</f>
+        <v>Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается</v>
+      </c>
       <c r="I17" s="38" t="s">
         <v>0</v>
       </c>
@@ -20887,7 +21068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I18" s="31" t="s">
         <v>0</v>
       </c>
@@ -20991,7 +21172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I19" s="31" t="s">
         <v>0</v>
       </c>
@@ -21095,7 +21276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I20" s="31" t="s">
         <v>0</v>
       </c>
@@ -21199,7 +21380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I21" s="31" t="s">
         <v>0</v>
       </c>
@@ -21303,7 +21484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I22" s="31" t="s">
         <v>0</v>
       </c>
@@ -21407,7 +21588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I23" s="31" t="s">
         <v>0</v>
       </c>
@@ -21511,7 +21692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I24" s="31" t="s">
         <v>0</v>
       </c>
@@ -21615,7 +21796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I25" s="31" t="s">
         <v>0</v>
       </c>
@@ -21719,7 +21900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I26" s="31" t="s">
         <v>0</v>
       </c>
@@ -21823,7 +22004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I27" s="31" t="s">
         <v>1</v>
       </c>
@@ -21927,7 +22108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I28" s="31" t="s">
         <v>1</v>
       </c>
@@ -22031,7 +22212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I29" s="31" t="s">
         <v>1</v>
       </c>
@@ -22135,7 +22316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I30" s="31" t="s">
         <v>1</v>
       </c>
@@ -22239,7 +22420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I31" s="31" t="s">
         <v>1</v>
       </c>
@@ -22343,7 +22524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I32" s="31" t="s">
         <v>1</v>
       </c>
@@ -22813,7 +22994,7 @@
   <dimension ref="A3:AP35"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C16" sqref="C16:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22823,7 +23004,7 @@
     <col min="3" max="3" width="23.85546875" customWidth="1"/>
     <col min="4" max="4" width="46.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
@@ -23314,11 +23495,37 @@
       </c>
     </row>
     <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="29">
+        <v>1</v>
+      </c>
+      <c r="F16" s="44" t="str">
+        <f>IF(E16=1, "Выбрана сплошная рассадка", IF(E16=2, "Выбрана рассадка через место","Ошибка, надо выбрать 1 или 2"))</f>
+        <v>Выбрана сплошная рассадка</v>
+      </c>
       <c r="H16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:42" ht="45" x14ac:dyDescent="0.25">
+      <c r="C17" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="29">
+        <v>1</v>
+      </c>
+      <c r="F17" s="44" t="str">
+        <f>IF(E17=1,"Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается",IF(E17=2,"Участники сидят через ряд, каждый второй ряд свободен",IF(E17=3,"Участники сидят два ряда через один, каждый третий ряд свободен","Ошибка, надо выбрать из 1, 2, 3")))</f>
+        <v>Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается</v>
+      </c>
       <c r="I17" s="38" t="s">
         <v>0</v>
       </c>
@@ -23422,7 +23629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I18" s="31" t="s">
         <v>0</v>
       </c>
@@ -23526,7 +23733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I19" s="31" t="s">
         <v>0</v>
       </c>
@@ -23630,7 +23837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I20" s="31" t="s">
         <v>0</v>
       </c>
@@ -23734,7 +23941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I21" s="31" t="s">
         <v>0</v>
       </c>
@@ -23838,7 +24045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I22" s="31" t="s">
         <v>0</v>
       </c>
@@ -23942,7 +24149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I23" s="31" t="s">
         <v>0</v>
       </c>
@@ -24046,7 +24253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I24" s="31" t="s">
         <v>0</v>
       </c>
@@ -24150,7 +24357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I25" s="31" t="s">
         <v>0</v>
       </c>
@@ -24254,7 +24461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I26" s="31" t="s">
         <v>1</v>
       </c>
@@ -24358,7 +24565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I27" s="31" t="s">
         <v>1</v>
       </c>
@@ -24462,7 +24669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I28" s="31" t="s">
         <v>1</v>
       </c>
@@ -24566,7 +24773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I29" s="31" t="s">
         <v>1</v>
       </c>
@@ -24670,7 +24877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I30" s="31" t="s">
         <v>1</v>
       </c>
@@ -24774,7 +24981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I31" s="31" t="s">
         <v>1</v>
       </c>
@@ -24878,7 +25085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I32" s="31" t="s">
         <v>1</v>
       </c>
@@ -25347,8 +25554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AP35"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25849,11 +26056,37 @@
       </c>
     </row>
     <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="29">
+        <v>1</v>
+      </c>
+      <c r="F16" s="44" t="str">
+        <f>IF(E16=1, "Выбрана сплошная рассадка", IF(E16=2, "Выбрана рассадка через место","Ошибка, надо выбрать 1 или 2"))</f>
+        <v>Выбрана сплошная рассадка</v>
+      </c>
       <c r="H16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:42" ht="60" x14ac:dyDescent="0.25">
+      <c r="C17" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="29">
+        <v>1</v>
+      </c>
+      <c r="F17" s="44" t="str">
+        <f>IF(E17=1,"Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается",IF(E17=2,"Участники сидят через ряд, каждый второй ряд свободен",IF(E17=3,"Участники сидят два ряда через один, каждый третий ряд свободен","Ошибка, надо выбрать из 1, 2, 3")))</f>
+        <v>Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается</v>
+      </c>
       <c r="I17" s="31" t="s">
         <v>1</v>
       </c>
@@ -25957,7 +26190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I18" s="31" t="s">
         <v>1</v>
       </c>
@@ -26061,7 +26294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I19" s="31" t="s">
         <v>1</v>
       </c>
@@ -26165,7 +26398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I20" s="31" t="s">
         <v>1</v>
       </c>
@@ -26269,7 +26502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I21" s="31" t="s">
         <v>1</v>
       </c>
@@ -26373,7 +26606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I22" s="31" t="s">
         <v>1</v>
       </c>
@@ -26477,7 +26710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I23" s="31" t="s">
         <v>1</v>
       </c>
@@ -26581,7 +26814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I24" s="31" t="s">
         <v>1</v>
       </c>
@@ -26685,7 +26918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I25" s="31" t="s">
         <v>1</v>
       </c>
@@ -26789,7 +27022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I26" s="31" t="s">
         <v>1</v>
       </c>
@@ -26893,7 +27126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I27" s="31" t="s">
         <v>1</v>
       </c>
@@ -26997,7 +27230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I28" s="31" t="s">
         <v>1</v>
       </c>
@@ -27101,7 +27334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I29" s="31" t="s">
         <v>1</v>
       </c>
@@ -27205,7 +27438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I30" s="31" t="s">
         <v>1</v>
       </c>
@@ -27309,7 +27542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I31" s="31" t="s">
         <v>1</v>
       </c>
@@ -27413,7 +27646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I32" s="31" t="s">
         <v>1</v>
       </c>
@@ -27883,7 +28116,7 @@
   <dimension ref="A3:AP35"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28384,11 +28617,37 @@
       </c>
     </row>
     <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="29">
+        <v>1</v>
+      </c>
+      <c r="F16" s="44" t="str">
+        <f>IF(E16=1, "Выбрана сплошная рассадка", IF(E16=2, "Выбрана рассадка через место","Ошибка, надо выбрать 1 или 2"))</f>
+        <v>Выбрана сплошная рассадка</v>
+      </c>
       <c r="H16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="9:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:42" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="29">
+        <v>1</v>
+      </c>
+      <c r="F17" s="44" t="str">
+        <f>IF(E17=1,"Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается",IF(E17=2,"Участники сидят через ряд, каждый второй ряд свободен",IF(E17=3,"Участники сидят два ряда через один, каждый третий ряд свободен","Ошибка, надо выбрать из 1, 2, 3")))</f>
+        <v>Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается</v>
+      </c>
       <c r="I17" s="1" t="s">
         <v>1</v>
       </c>
@@ -28492,7 +28751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I18" s="3" t="s">
         <v>0</v>
       </c>
@@ -28596,7 +28855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I19" s="3" t="s">
         <v>0</v>
       </c>
@@ -28700,7 +28959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I20" s="5" t="s">
         <v>1</v>
       </c>
@@ -28804,7 +29063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I21" s="5" t="s">
         <v>1</v>
       </c>
@@ -28908,7 +29167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I22" s="5" t="s">
         <v>1</v>
       </c>
@@ -29012,7 +29271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I23" s="5" t="s">
         <v>1</v>
       </c>
@@ -29116,7 +29375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I24" s="5" t="s">
         <v>1</v>
       </c>
@@ -29220,7 +29479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I25" s="5" t="s">
         <v>1</v>
       </c>
@@ -29324,7 +29583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I26" s="5" t="s">
         <v>1</v>
       </c>
@@ -29428,7 +29687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I27" s="5" t="s">
         <v>1</v>
       </c>
@@ -29532,7 +29791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I28" s="5" t="s">
         <v>1</v>
       </c>
@@ -29636,7 +29895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I29" s="5" t="s">
         <v>1</v>
       </c>
@@ -29740,7 +29999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I30" s="5" t="s">
         <v>1</v>
       </c>
@@ -29844,7 +30103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I31" s="5" t="s">
         <v>1</v>
       </c>
@@ -29948,7 +30207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I32" s="5" t="s">
         <v>1</v>
       </c>
@@ -30418,7 +30677,7 @@
   <dimension ref="A3:AP35"/>
   <sheetViews>
     <sheetView topLeftCell="A6" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C16" sqref="C16:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30919,11 +31178,37 @@
       </c>
     </row>
     <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="29">
+        <v>1</v>
+      </c>
+      <c r="F16" s="44" t="str">
+        <f>IF(E16=1, "Выбрана сплошная рассадка", IF(E16=2, "Выбрана рассадка через место","Ошибка, надо выбрать 1 или 2"))</f>
+        <v>Выбрана сплошная рассадка</v>
+      </c>
       <c r="H16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:42" ht="60" x14ac:dyDescent="0.25">
+      <c r="C17" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="29">
+        <v>1</v>
+      </c>
+      <c r="F17" s="44" t="str">
+        <f>IF(E17=1,"Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается",IF(E17=2,"Участники сидят через ряд, каждый второй ряд свободен",IF(E17=3,"Участники сидят два ряда через один, каждый третий ряд свободен","Ошибка, надо выбрать из 1, 2, 3")))</f>
+        <v>Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается</v>
+      </c>
       <c r="I17" s="31" t="s">
         <v>1</v>
       </c>
@@ -31027,7 +31312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I18" s="33" t="s">
         <v>1</v>
       </c>
@@ -31131,7 +31416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I19" s="33" t="s">
         <v>0</v>
       </c>
@@ -31235,7 +31520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I20" s="31" t="s">
         <v>1</v>
       </c>
@@ -31339,7 +31624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I21" s="31" t="s">
         <v>1</v>
       </c>
@@ -31443,7 +31728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I22" s="31" t="s">
         <v>1</v>
       </c>
@@ -31547,7 +31832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I23" s="31" t="s">
         <v>1</v>
       </c>
@@ -31651,7 +31936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I24" s="31" t="s">
         <v>1</v>
       </c>
@@ -31755,7 +32040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I25" s="31" t="s">
         <v>1</v>
       </c>
@@ -31859,7 +32144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I26" s="31" t="s">
         <v>1</v>
       </c>
@@ -31963,7 +32248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I27" s="31" t="s">
         <v>1</v>
       </c>
@@ -32067,7 +32352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I28" s="31" t="s">
         <v>1</v>
       </c>
@@ -32171,7 +32456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I29" s="31" t="s">
         <v>1</v>
       </c>
@@ -32275,7 +32560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I30" s="31" t="s">
         <v>1</v>
       </c>
@@ -32379,7 +32664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I31" s="31" t="s">
         <v>1</v>
       </c>
@@ -32483,7 +32768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I32" s="31" t="s">
         <v>1</v>
       </c>
@@ -32953,7 +33238,7 @@
   <dimension ref="A3:AP35"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C16" sqref="C16:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33454,11 +33739,37 @@
       </c>
     </row>
     <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="29">
+        <v>1</v>
+      </c>
+      <c r="F16" s="44" t="str">
+        <f>IF(E16=1, "Выбрана сплошная рассадка", IF(E16=2, "Выбрана рассадка через место","Ошибка, надо выбрать 1 или 2"))</f>
+        <v>Выбрана сплошная рассадка</v>
+      </c>
       <c r="H16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:42" ht="60" x14ac:dyDescent="0.25">
+      <c r="C17" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="29">
+        <v>1</v>
+      </c>
+      <c r="F17" s="44" t="str">
+        <f>IF(E17=1,"Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается",IF(E17=2,"Участники сидят через ряд, каждый второй ряд свободен",IF(E17=3,"Участники сидят два ряда через один, каждый третий ряд свободен","Ошибка, надо выбрать из 1, 2, 3")))</f>
+        <v>Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается</v>
+      </c>
       <c r="I17" s="38" t="s">
         <v>1</v>
       </c>
@@ -33562,7 +33873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I18" s="31" t="s">
         <v>0</v>
       </c>
@@ -33666,7 +33977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I19" s="33" t="s">
         <v>0</v>
       </c>
@@ -33770,7 +34081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I20" s="31" t="s">
         <v>1</v>
       </c>
@@ -33874,7 +34185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I21" s="31" t="s">
         <v>0</v>
       </c>
@@ -33978,7 +34289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I22" s="31" t="s">
         <v>1</v>
       </c>
@@ -34082,7 +34393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I23" s="31" t="s">
         <v>1</v>
       </c>
@@ -34186,7 +34497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I24" s="31" t="s">
         <v>1</v>
       </c>
@@ -34290,7 +34601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I25" s="31" t="s">
         <v>1</v>
       </c>
@@ -34394,7 +34705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I26" s="31" t="s">
         <v>1</v>
       </c>
@@ -34498,7 +34809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I27" s="31" t="s">
         <v>1</v>
       </c>
@@ -34602,7 +34913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I28" s="31" t="s">
         <v>1</v>
       </c>
@@ -34706,7 +35017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I29" s="31" t="s">
         <v>1</v>
       </c>
@@ -34810,7 +35121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I30" s="31" t="s">
         <v>1</v>
       </c>
@@ -34914,7 +35225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I31" s="31" t="s">
         <v>1</v>
       </c>
@@ -35018,7 +35329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I32" s="31" t="s">
         <v>1</v>
       </c>
@@ -35488,7 +35799,7 @@
   <dimension ref="A3:AP35"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C16" sqref="C16:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35989,11 +36300,37 @@
       </c>
     </row>
     <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="29">
+        <v>1</v>
+      </c>
+      <c r="F16" s="44" t="str">
+        <f>IF(E16=1, "Выбрана сплошная рассадка", IF(E16=2, "Выбрана рассадка через место","Ошибка, надо выбрать 1 или 2"))</f>
+        <v>Выбрана сплошная рассадка</v>
+      </c>
       <c r="H16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:42" ht="60" x14ac:dyDescent="0.25">
+      <c r="C17" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="29">
+        <v>1</v>
+      </c>
+      <c r="F17" s="44" t="str">
+        <f>IF(E17=1,"Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается",IF(E17=2,"Участники сидят через ряд, каждый второй ряд свободен",IF(E17=3,"Участники сидят два ряда через один, каждый третий ряд свободен","Ошибка, надо выбрать из 1, 2, 3")))</f>
+        <v>Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается</v>
+      </c>
       <c r="I17" s="38" t="s">
         <v>1</v>
       </c>
@@ -36097,7 +36434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I18" s="31" t="s">
         <v>1</v>
       </c>
@@ -36201,7 +36538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I19" s="31" t="s">
         <v>1</v>
       </c>
@@ -36305,7 +36642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I20" s="31" t="s">
         <v>1</v>
       </c>
@@ -36409,7 +36746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I21" s="31" t="s">
         <v>1</v>
       </c>
@@ -36513,7 +36850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I22" s="31" t="s">
         <v>1</v>
       </c>
@@ -36617,7 +36954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I23" s="31" t="s">
         <v>1</v>
       </c>
@@ -36721,7 +37058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I24" s="31" t="s">
         <v>1</v>
       </c>
@@ -36825,7 +37162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I25" s="31" t="s">
         <v>1</v>
       </c>
@@ -36929,7 +37266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I26" s="31" t="s">
         <v>1</v>
       </c>
@@ -37033,7 +37370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I27" s="31" t="s">
         <v>1</v>
       </c>
@@ -37137,7 +37474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I28" s="31" t="s">
         <v>0</v>
       </c>
@@ -37241,7 +37578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I29" s="33" t="s">
         <v>1</v>
       </c>
@@ -37345,7 +37682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I30" s="31" t="s">
         <v>0</v>
       </c>
@@ -37449,7 +37786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I31" s="31" t="s">
         <v>1</v>
       </c>
@@ -37553,7 +37890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I32" s="31" t="s">
         <v>1</v>
       </c>
@@ -38023,7 +38360,7 @@
   <dimension ref="A3:AP35"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C16" sqref="C16:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38524,11 +38861,37 @@
       </c>
     </row>
     <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="29">
+        <v>1</v>
+      </c>
+      <c r="F16" s="44" t="str">
+        <f>IF(E16=1, "Выбрана сплошная рассадка", IF(E16=2, "Выбрана рассадка через место","Ошибка, надо выбрать 1 или 2"))</f>
+        <v>Выбрана сплошная рассадка</v>
+      </c>
       <c r="H16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:42" ht="60" x14ac:dyDescent="0.25">
+      <c r="C17" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="29">
+        <v>1</v>
+      </c>
+      <c r="F17" s="44" t="str">
+        <f>IF(E17=1,"Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается",IF(E17=2,"Участники сидят через ряд, каждый второй ряд свободен",IF(E17=3,"Участники сидят два ряда через один, каждый третий ряд свободен","Ошибка, надо выбрать из 1, 2, 3")))</f>
+        <v>Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается</v>
+      </c>
       <c r="I17" s="38" t="s">
         <v>0</v>
       </c>
@@ -38632,7 +38995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I18" s="31" t="s">
         <v>0</v>
       </c>
@@ -38736,7 +39099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I19" s="31" t="s">
         <v>0</v>
       </c>
@@ -38840,7 +39203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I20" s="31" t="s">
         <v>0</v>
       </c>
@@ -38944,7 +39307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I21" s="31" t="s">
         <v>0</v>
       </c>
@@ -39048,7 +39411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I22" s="31" t="s">
         <v>0</v>
       </c>
@@ -39152,7 +39515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I23" s="31" t="s">
         <v>0</v>
       </c>
@@ -39256,7 +39619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I24" s="31" t="s">
         <v>0</v>
       </c>
@@ -39360,7 +39723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I25" s="31" t="s">
         <v>0</v>
       </c>
@@ -39464,7 +39827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I26" s="31" t="s">
         <v>1</v>
       </c>
@@ -39568,7 +39931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I27" s="31" t="s">
         <v>1</v>
       </c>
@@ -39672,7 +40035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I28" s="31" t="s">
         <v>1</v>
       </c>
@@ -39776,7 +40139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I29" s="31" t="s">
         <v>1</v>
       </c>
@@ -39880,7 +40243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I30" s="31" t="s">
         <v>1</v>
       </c>
@@ -39984,7 +40347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I31" s="31" t="s">
         <v>1</v>
       </c>
@@ -40088,7 +40451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I32" s="31" t="s">
         <v>1</v>
       </c>
@@ -40558,7 +40921,7 @@
   <dimension ref="A3:AP35"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C16" sqref="C16:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41059,11 +41422,37 @@
       </c>
     </row>
     <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="29">
+        <v>1</v>
+      </c>
+      <c r="F16" s="44" t="str">
+        <f>IF(E16=1, "Выбрана сплошная рассадка", IF(E16=2, "Выбрана рассадка через место","Ошибка, надо выбрать 1 или 2"))</f>
+        <v>Выбрана сплошная рассадка</v>
+      </c>
       <c r="H16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:42" ht="60" x14ac:dyDescent="0.25">
+      <c r="C17" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="29">
+        <v>1</v>
+      </c>
+      <c r="F17" s="44" t="str">
+        <f>IF(E17=1,"Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается",IF(E17=2,"Участники сидят через ряд, каждый второй ряд свободен",IF(E17=3,"Участники сидят два ряда через один, каждый третий ряд свободен","Ошибка, надо выбрать из 1, 2, 3")))</f>
+        <v>Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается</v>
+      </c>
       <c r="I17" s="38" t="s">
         <v>0</v>
       </c>
@@ -41167,7 +41556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I18" s="31" t="s">
         <v>0</v>
       </c>
@@ -41271,7 +41660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I19" s="31" t="s">
         <v>0</v>
       </c>
@@ -41375,7 +41764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I20" s="31" t="s">
         <v>0</v>
       </c>
@@ -41479,7 +41868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I21" s="31" t="s">
         <v>0</v>
       </c>
@@ -41583,7 +41972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I22" s="31" t="s">
         <v>0</v>
       </c>
@@ -41687,7 +42076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I23" s="31" t="s">
         <v>0</v>
       </c>
@@ -41791,7 +42180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I24" s="31" t="s">
         <v>0</v>
       </c>
@@ -41895,7 +42284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I25" s="31" t="s">
         <v>0</v>
       </c>
@@ -41999,7 +42388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I26" s="31" t="s">
         <v>1</v>
       </c>
@@ -42103,7 +42492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I27" s="31" t="s">
         <v>1</v>
       </c>
@@ -42207,7 +42596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I28" s="31" t="s">
         <v>1</v>
       </c>
@@ -42311,7 +42700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I29" s="31" t="s">
         <v>1</v>
       </c>
@@ -42415,7 +42804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I30" s="31" t="s">
         <v>1</v>
       </c>
@@ -42519,7 +42908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I31" s="31" t="s">
         <v>1</v>
       </c>
@@ -42623,7 +43012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I32" s="31" t="s">
         <v>1</v>
       </c>
@@ -43093,7 +43482,7 @@
   <dimension ref="A3:AP35"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C16" sqref="C16:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43594,11 +43983,37 @@
       </c>
     </row>
     <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="29">
+        <v>1</v>
+      </c>
+      <c r="F16" s="44" t="str">
+        <f>IF(E16=1, "Выбрана сплошная рассадка", IF(E16=2, "Выбрана рассадка через место","Ошибка, надо выбрать 1 или 2"))</f>
+        <v>Выбрана сплошная рассадка</v>
+      </c>
       <c r="H16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:42" ht="60" x14ac:dyDescent="0.25">
+      <c r="C17" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="29">
+        <v>1</v>
+      </c>
+      <c r="F17" s="44" t="str">
+        <f>IF(E17=1,"Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается",IF(E17=2,"Участники сидят через ряд, каждый второй ряд свободен",IF(E17=3,"Участники сидят два ряда через один, каждый третий ряд свободен","Ошибка, надо выбрать из 1, 2, 3")))</f>
+        <v>Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается</v>
+      </c>
       <c r="I17" s="38" t="s">
         <v>0</v>
       </c>
@@ -43702,7 +44117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I18" s="31" t="s">
         <v>0</v>
       </c>
@@ -43806,7 +44221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I19" s="31" t="s">
         <v>0</v>
       </c>
@@ -43910,7 +44325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I20" s="31" t="s">
         <v>0</v>
       </c>
@@ -44014,7 +44429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I21" s="31" t="s">
         <v>0</v>
       </c>
@@ -44118,7 +44533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I22" s="31" t="s">
         <v>0</v>
       </c>
@@ -44222,7 +44637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I23" s="31" t="s">
         <v>0</v>
       </c>
@@ -44326,7 +44741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I24" s="31" t="s">
         <v>0</v>
       </c>
@@ -44430,7 +44845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I25" s="31" t="s">
         <v>0</v>
       </c>
@@ -44534,7 +44949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I26" s="31" t="s">
         <v>0</v>
       </c>
@@ -44638,7 +45053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I27" s="31" t="s">
         <v>1</v>
       </c>
@@ -44742,7 +45157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I28" s="31" t="s">
         <v>1</v>
       </c>
@@ -44846,7 +45261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I29" s="31" t="s">
         <v>1</v>
       </c>
@@ -44950,7 +45365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I30" s="31" t="s">
         <v>1</v>
       </c>
@@ -45054,7 +45469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I31" s="31" t="s">
         <v>1</v>
       </c>
@@ -45158,7 +45573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I32" s="31" t="s">
         <v>1</v>
       </c>
@@ -45627,8 +46042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AP35"/>
   <sheetViews>
-    <sheetView topLeftCell="F4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46129,11 +46544,37 @@
       </c>
     </row>
     <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="29">
+        <v>1</v>
+      </c>
+      <c r="F16" s="44" t="str">
+        <f>IF(E16=1, "Выбрана сплошная рассадка", IF(E16=2, "Выбрана рассадка через место","Ошибка, надо выбрать 1 или 2"))</f>
+        <v>Выбрана сплошная рассадка</v>
+      </c>
       <c r="H16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:42" ht="60" x14ac:dyDescent="0.25">
+      <c r="C17" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="29">
+        <v>1</v>
+      </c>
+      <c r="F17" s="44" t="str">
+        <f>IF(E17=1,"Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается",IF(E17=2,"Участники сидят через ряд, каждый второй ряд свободен",IF(E17=3,"Участники сидят два ряда через один, каждый третий ряд свободен","Ошибка, надо выбрать из 1, 2, 3")))</f>
+        <v>Участники сидят на каждом ряду, технических рядов для прохода организаторов не остается</v>
+      </c>
       <c r="I17" s="38" t="s">
         <v>0</v>
       </c>
@@ -46237,7 +46678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I18" s="31" t="s">
         <v>0</v>
       </c>
@@ -46341,7 +46782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I19" s="31" t="s">
         <v>0</v>
       </c>
@@ -46445,7 +46886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I20" s="31" t="s">
         <v>0</v>
       </c>
@@ -46549,7 +46990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I21" s="31" t="s">
         <v>0</v>
       </c>
@@ -46653,7 +47094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I22" s="31" t="s">
         <v>0</v>
       </c>
@@ -46757,7 +47198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I23" s="31" t="s">
         <v>0</v>
       </c>
@@ -46861,7 +47302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I24" s="31" t="s">
         <v>0</v>
       </c>
@@ -46965,7 +47406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I25" s="31" t="s">
         <v>0</v>
       </c>
@@ -47069,7 +47510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I26" s="31" t="s">
         <v>0</v>
       </c>
@@ -47173,7 +47614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I27" s="31" t="s">
         <v>0</v>
       </c>
@@ -47277,7 +47718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I28" s="31" t="s">
         <v>0</v>
       </c>
@@ -47381,7 +47822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I29" s="31" t="s">
         <v>0</v>
       </c>
@@ -47485,7 +47926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I30" s="31" t="s">
         <v>0</v>
       </c>
@@ -47589,7 +48030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I31" s="31" t="s">
         <v>1</v>
       </c>
@@ -47693,7 +48134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="9:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:42" x14ac:dyDescent="0.25">
       <c r="I32" s="31" t="s">
         <v>1</v>
       </c>

</xml_diff>